<commit_message>
Intermediate survey speed changes
</commit_message>
<xml_diff>
--- a/app/config/tables/gridScreen/forms/gridScreen/gridScreen.xlsx
+++ b/app/config/tables/gridScreen/forms/gridScreen/gridScreen.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\toolsuite\app-designer\app\config\tables\gridScreen\forms\gridScreen\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1924" yWindow="6362" windowWidth="25815" windowHeight="16220" tabRatio="439" activeTab="2"/>
+    <workbookView xWindow="1620" yWindow="3520" windowWidth="33120" windowHeight="16100" tabRatio="439" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -339,15 +334,6 @@
     <t>Target_get_total</t>
   </si>
   <si>
-    <t>data('QFC_item_1')+data('QFC_item_2')+data('QFC_item_3')+data('QFC_item_4')+data('QFC_item_5')+data('QFC_item_6')</t>
-  </si>
-  <si>
-    <t>data('Safeway_item_1')+data('Safeway_item_2')+data('Safeway_item_3')+data('Safeway_item_4')+data('Safeway_item_5')+data('Safeway_item_6')</t>
-  </si>
-  <si>
-    <t>data('Target_item_1')+data('Target_item_2')+data('Target_item_3')+data('Target_item_4')+data('Target_item_5')+data('Target_item_6')</t>
-  </si>
-  <si>
     <t>Which store will you visit?</t>
   </si>
   <si>
@@ -403,12 +389,36 @@
   </si>
   <si>
     <t>display.hint.text</t>
+  </si>
+  <si>
+    <t>(parseInt(data('QFC_item_1')) ? parseInt(data('QFC_item_1')) : 0) + 
+(parseInt(data('QFC_item_2')) ? parseInt(data('QFC_item_2')) : 0) +
+(parseInt(data('QFC_item_3')) ? parseInt(data('QFC_item_3')) : 0) +
+(parseInt(data('QFC_item_4')) ? parseInt(data('QFC_item_4')) : 0) +
+(parseInt(data('QFC_item_5')) ? parseInt(data('QFC_item_5')) : 0) +
+(parseInt(data('QFC_item_6')) ? parseInt(data('QFC_item_6')) : 0)</t>
+  </si>
+  <si>
+    <t>(parseInt(data('Safeway_item_1')) ? parseInt(data('Safeway_item_1')) : 0) + 
+(parseInt(data('Safeway_item_2')) ? parseInt(data('Safeway_item_2')) : 0) +
+(parseInt(data('Safeway_item_3')) ? parseInt(data('Safeway_item_3')) : 0) +
+(parseInt(data('Safeway_item_4')) ? parseInt(data('Safeway_item_4')) : 0) +
+(parseInt(data('Safeway_item_5')) ? parseInt(data('Safeway_item_5')) : 0) +
+(parseInt(data('Safeway_item_6')) ? parseInt(data('Safeway_item_6')) : 0)</t>
+  </si>
+  <si>
+    <t>(parseInt(data('Target_item_1')) ? parseInt(data('Target_item_1')) : 0) + 
+(parseInt(data('Target_item_2')) ? parseInt(data('Target_item_2')) : 0) +
+(parseInt(data('Target_item_3')) ? parseInt(data('Target_item_3')) : 0) +
+(parseInt(data('Target_item_4')) ? parseInt(data('Target_item_4')) : 0) +
+(parseInt(data('Target_item_5')) ? parseInt(data('Target_item_5')) : 0) +
+(parseInt(data('Target_item_6')) ? parseInt(data('Target_item_6')) : 0)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -563,7 +573,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -615,7 +625,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -847,23 +857,23 @@
       <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="12.8" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="13.625" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
     <col min="3" max="3" width="11.5" customWidth="1"/>
-    <col min="4" max="4" width="13.125" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" customWidth="1"/>
     <col min="5" max="5" width="17.5" customWidth="1"/>
     <col min="6" max="6" width="67" customWidth="1"/>
-    <col min="7" max="7" width="14.625" customWidth="1"/>
-    <col min="8" max="8" width="16.375" customWidth="1"/>
-    <col min="9" max="9" width="26.375" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
+    <col min="9" max="9" width="26.33203125" customWidth="1"/>
     <col min="10" max="10" width="9.5" customWidth="1"/>
     <col min="11" max="11" width="40" customWidth="1"/>
-    <col min="12" max="12" width="27.875" customWidth="1"/>
-    <col min="13" max="22" width="23.625" customWidth="1"/>
+    <col min="12" max="12" width="27.83203125" customWidth="1"/>
+    <col min="13" max="22" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="17.5" customHeight="1">
       <c r="A1" s="9"/>
       <c r="B1" s="9" t="s">
         <v>51</v>
@@ -878,7 +888,7 @@
         <v>53</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G1" s="10" t="s">
         <v>0</v>
@@ -887,22 +897,22 @@
         <v>2</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="J1" s="10" t="s">
         <v>49</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="L1" s="10" t="s">
         <v>10</v>
       </c>
       <c r="M1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="17.5" customHeight="1">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -910,10 +920,10 @@
         <v>55</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>109</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>112</v>
       </c>
       <c r="G2" s="7"/>
       <c r="H2" s="5"/>
@@ -922,7 +932,7 @@
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
     </row>
-    <row r="3" spans="1:13" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="17.5" customHeight="1">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
@@ -943,7 +953,7 @@
       </c>
       <c r="L3" s="8"/>
     </row>
-    <row r="4" spans="1:13" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="17.5" customHeight="1">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -964,7 +974,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="17.5" customHeight="1">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -985,7 +995,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="17.5" customHeight="1">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -1006,7 +1016,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="17.5" customHeight="1">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -1027,7 +1037,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="17.5" customHeight="1">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -1048,7 +1058,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="17.5" customHeight="1">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -1069,7 +1079,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="17.5" customHeight="1">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -1090,7 +1100,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="17.5" customHeight="1">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -1111,7 +1121,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="17.5" customHeight="1">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -1132,7 +1142,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="17.5" customHeight="1">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -1153,7 +1163,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="17.55" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="17.5" hidden="1" customHeight="1">
       <c r="G14" s="8" t="s">
         <v>9</v>
       </c>
@@ -1166,7 +1176,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="17.55" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="17.5" hidden="1" customHeight="1">
       <c r="G15" s="8" t="s">
         <v>9</v>
       </c>
@@ -1179,7 +1189,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="17.55" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="17.5" hidden="1" customHeight="1">
       <c r="G16" s="8" t="s">
         <v>9</v>
       </c>
@@ -1192,7 +1202,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="3:13" s="11" customFormat="1" ht="17.55" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:13" s="11" customFormat="1" ht="17.5" hidden="1" customHeight="1">
       <c r="G17" s="12" t="s">
         <v>95</v>
       </c>
@@ -1206,7 +1216,7 @@
       </c>
       <c r="M17" s="8"/>
     </row>
-    <row r="18" spans="3:13" ht="17.55" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:13" ht="17.5" hidden="1" customHeight="1">
       <c r="G18" s="8" t="s">
         <v>9</v>
       </c>
@@ -1219,7 +1229,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="19" spans="3:13" ht="17.55" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:13" ht="17.5" hidden="1" customHeight="1">
       <c r="G19" s="8" t="s">
         <v>9</v>
       </c>
@@ -1232,7 +1242,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="3:13" ht="17.55" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:13" ht="17.5" hidden="1" customHeight="1">
       <c r="G20" s="8" t="s">
         <v>9</v>
       </c>
@@ -1245,7 +1255,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="3:13" ht="17.55" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:13" ht="17.5" hidden="1" customHeight="1">
       <c r="G21" s="8" t="s">
         <v>9</v>
       </c>
@@ -1258,7 +1268,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="3:13" ht="17.55" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:13" ht="17.5" hidden="1" customHeight="1">
       <c r="G22" s="8" t="s">
         <v>9</v>
       </c>
@@ -1271,7 +1281,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="3:13" ht="17.55" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:13" ht="17.5" hidden="1" customHeight="1">
       <c r="G23" s="8" t="s">
         <v>9</v>
       </c>
@@ -1284,7 +1294,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="3:13" ht="17.55" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:13" ht="17.5" hidden="1" customHeight="1">
       <c r="G24" s="8" t="s">
         <v>9</v>
       </c>
@@ -1297,7 +1307,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="3:13" s="11" customFormat="1" ht="17.55" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:13" s="11" customFormat="1" ht="17.5" hidden="1" customHeight="1">
       <c r="G25" s="12" t="s">
         <v>95</v>
       </c>
@@ -1311,7 +1321,7 @@
       </c>
       <c r="M25" s="8"/>
     </row>
-    <row r="26" spans="3:13" ht="17.55" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:13" ht="17.5" hidden="1" customHeight="1">
       <c r="G26" s="8" t="s">
         <v>9</v>
       </c>
@@ -1324,7 +1334,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="3:13" ht="17.55" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:13" ht="17.5" hidden="1" customHeight="1">
       <c r="G27" s="8" t="s">
         <v>9</v>
       </c>
@@ -1337,7 +1347,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="28" spans="3:13" ht="17.55" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:13" ht="17.5" hidden="1" customHeight="1">
       <c r="G28" s="8" t="s">
         <v>9</v>
       </c>
@@ -1350,7 +1360,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="3:13" ht="17.55" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:13" ht="17.5" hidden="1" customHeight="1">
       <c r="G29" s="8" t="s">
         <v>9</v>
       </c>
@@ -1363,7 +1373,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="3:13" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:13" ht="17.5" customHeight="1">
       <c r="G30" s="8" t="s">
         <v>9</v>
       </c>
@@ -1376,7 +1386,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="3:13" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:13" ht="17.5" customHeight="1">
       <c r="G31" s="8" t="s">
         <v>9</v>
       </c>
@@ -1389,7 +1399,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="32" spans="3:13" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:13" ht="17.5" customHeight="1">
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
@@ -1406,7 +1416,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="3:13" s="11" customFormat="1" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:13" s="11" customFormat="1" ht="17.5" customHeight="1">
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
@@ -1424,7 +1434,7 @@
       </c>
       <c r="M33" s="12"/>
     </row>
-    <row r="34" spans="3:13" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:13" ht="17.5" customHeight="1">
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
@@ -1441,7 +1451,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="35" spans="3:13" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:13" ht="17.5" customHeight="1">
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
@@ -1453,13 +1463,13 @@
         <v>80</v>
       </c>
       <c r="I35" s="12" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="J35" s="8" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="36" spans="3:13" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:13" ht="17.5" customHeight="1">
       <c r="C36" s="8"/>
       <c r="D36" t="s">
         <v>8</v>
@@ -1471,89 +1481,89 @@
       <c r="I36" s="8"/>
       <c r="J36" s="8"/>
     </row>
-    <row r="37" spans="3:13" s="11" customFormat="1" ht="17.55" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:13" s="11" customFormat="1" ht="17.5" hidden="1" customHeight="1">
       <c r="E37" s="11" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G37" s="15" t="s">
         <v>6</v>
       </c>
       <c r="H37" s="5"/>
       <c r="I37" s="16" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="J37" s="7"/>
     </row>
-    <row r="38" spans="3:13" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="3:13" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="3:13" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="3:13" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="3:13" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="3:13" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="3:13" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="3:13" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="3:13" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="3:13" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="3:13" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="50" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="65" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="66" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="67" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="68" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="70" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="72" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="73" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="74" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="76" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="77" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="78" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="79" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="81" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="82" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="83" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="84" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="85" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="86" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="87" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="88" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="89" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="90" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="91" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="92" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="93" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="94" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="95" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="96" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="97" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="98" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="99" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="100" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="101" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="102" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="103" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="104" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="105" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="106" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="107" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="3:13" ht="17.5" customHeight="1"/>
+    <row r="39" spans="3:13" ht="17.5" customHeight="1"/>
+    <row r="40" spans="3:13" ht="17.5" customHeight="1"/>
+    <row r="41" spans="3:13" ht="17.5" customHeight="1"/>
+    <row r="42" spans="3:13" ht="17.5" customHeight="1"/>
+    <row r="43" spans="3:13" ht="17.5" customHeight="1"/>
+    <row r="44" spans="3:13" ht="17.5" customHeight="1"/>
+    <row r="45" spans="3:13" ht="17.5" customHeight="1"/>
+    <row r="46" spans="3:13" ht="17.5" customHeight="1"/>
+    <row r="47" spans="3:13" ht="17.5" customHeight="1"/>
+    <row r="48" spans="3:13" ht="17.5" customHeight="1"/>
+    <row r="49" ht="17.5" customHeight="1"/>
+    <row r="50" ht="17.5" customHeight="1"/>
+    <row r="51" ht="17.5" customHeight="1"/>
+    <row r="52" ht="17.5" customHeight="1"/>
+    <row r="53" ht="17.5" customHeight="1"/>
+    <row r="54" ht="17.5" customHeight="1"/>
+    <row r="55" ht="17.5" customHeight="1"/>
+    <row r="56" ht="17.5" customHeight="1"/>
+    <row r="57" ht="17.5" customHeight="1"/>
+    <row r="58" ht="17.5" customHeight="1"/>
+    <row r="59" ht="17.5" customHeight="1"/>
+    <row r="60" ht="17.5" customHeight="1"/>
+    <row r="61" ht="17.5" customHeight="1"/>
+    <row r="62" ht="17.5" customHeight="1"/>
+    <row r="63" ht="17.5" customHeight="1"/>
+    <row r="64" ht="17.5" customHeight="1"/>
+    <row r="65" ht="17.5" customHeight="1"/>
+    <row r="66" ht="17.5" customHeight="1"/>
+    <row r="67" ht="17.5" customHeight="1"/>
+    <row r="68" ht="17.5" customHeight="1"/>
+    <row r="69" ht="17.5" customHeight="1"/>
+    <row r="70" ht="17.5" customHeight="1"/>
+    <row r="71" ht="17.5" customHeight="1"/>
+    <row r="72" ht="17.5" customHeight="1"/>
+    <row r="73" ht="17.5" customHeight="1"/>
+    <row r="74" ht="17.5" customHeight="1"/>
+    <row r="75" ht="17.5" customHeight="1"/>
+    <row r="76" ht="17.5" customHeight="1"/>
+    <row r="77" ht="17.5" customHeight="1"/>
+    <row r="78" ht="17.5" customHeight="1"/>
+    <row r="79" ht="17.5" customHeight="1"/>
+    <row r="80" ht="17.5" customHeight="1"/>
+    <row r="81" ht="17.5" customHeight="1"/>
+    <row r="82" ht="17.5" customHeight="1"/>
+    <row r="83" ht="17.5" customHeight="1"/>
+    <row r="84" ht="17.5" customHeight="1"/>
+    <row r="85" ht="17.5" customHeight="1"/>
+    <row r="86" ht="17.5" customHeight="1"/>
+    <row r="87" ht="17.5" customHeight="1"/>
+    <row r="88" ht="17.5" customHeight="1"/>
+    <row r="89" ht="17.5" customHeight="1"/>
+    <row r="90" ht="17.5" customHeight="1"/>
+    <row r="91" ht="17.5" customHeight="1"/>
+    <row r="92" ht="17.5" customHeight="1"/>
+    <row r="93" ht="17.5" customHeight="1"/>
+    <row r="94" ht="17.5" customHeight="1"/>
+    <row r="95" ht="17.5" customHeight="1"/>
+    <row r="96" ht="17.5" customHeight="1"/>
+    <row r="97" ht="17.5" customHeight="1"/>
+    <row r="98" ht="17.5" customHeight="1"/>
+    <row r="99" ht="17.5" customHeight="1"/>
+    <row r="100" ht="17.5" customHeight="1"/>
+    <row r="101" ht="17.5" customHeight="1"/>
+    <row r="102" ht="17.5" customHeight="1"/>
+    <row r="103" ht="17.5" customHeight="1"/>
+    <row r="104" ht="17.5" customHeight="1"/>
+    <row r="105" ht="17.5" customHeight="1"/>
+    <row r="106" ht="17.5" customHeight="1"/>
+    <row r="107" ht="17.5" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1568,17 +1578,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="12.8" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="25.625" customWidth="1"/>
-    <col min="2" max="2" width="49.5" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" customWidth="1"/>
+    <col min="2" max="2" width="57.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="17.5" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>47</v>
       </c>
@@ -1586,7 +1596,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="17.5" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1594,28 +1604,28 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="80" customHeight="1">
       <c r="A3" t="s">
         <v>93</v>
       </c>
       <c r="B3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="84" customHeight="1">
       <c r="A4" t="s">
         <v>101</v>
       </c>
       <c r="B4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="91" customHeight="1">
       <c r="A5" t="s">
         <v>102</v>
       </c>
       <c r="B5" t="s">
-        <v>105</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1632,18 +1642,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="12.8" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.875" customWidth="1"/>
-    <col min="2" max="2" width="18.125" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" customWidth="1"/>
     <col min="3" max="3" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="17.5" customHeight="1">
       <c r="A1" t="s">
         <v>45</v>
       </c>
@@ -1651,10 +1661,10 @@
         <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="17.5" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -1665,7 +1675,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="17.5" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -1676,7 +1686,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="17.5" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -1687,7 +1697,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="17.5" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -1698,7 +1708,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="17.5" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -1709,7 +1719,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="17.5" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -1720,7 +1730,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="17.5" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -1731,7 +1741,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="17.5" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -1742,7 +1752,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="17.5" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -1753,8 +1763,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="17.5" customHeight="1"/>
+    <row r="12" spans="1:3" ht="17.5" customHeight="1">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -1765,7 +1775,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="17.5" customHeight="1">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -1776,7 +1786,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="17.5" customHeight="1">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -1787,7 +1797,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="17.5" customHeight="1">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -1798,7 +1808,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="17.5" customHeight="1">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -1809,7 +1819,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="17.5" customHeight="1">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -1820,7 +1830,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="17.5" customHeight="1">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -1831,7 +1841,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="17.5" customHeight="1">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -1842,7 +1852,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="17.5" customHeight="1">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -1853,7 +1863,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="17.5" customHeight="1">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -1864,8 +1874,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="17.5" customHeight="1"/>
+    <row r="23" spans="1:3" ht="17.5" customHeight="1">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -1876,7 +1886,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="17.5" customHeight="1">
       <c r="A24" t="s">
         <v>39</v>
       </c>
@@ -1887,8 +1897,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="1:3" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="17.5" customHeight="1"/>
+    <row r="26" spans="1:3" ht="17.5" customHeight="1">
       <c r="A26" s="11" t="s">
         <v>79</v>
       </c>
@@ -1899,7 +1909,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="12.75" customHeight="1">
       <c r="A27" s="11" t="s">
         <v>79</v>
       </c>
@@ -1910,7 +1920,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="12.75" customHeight="1">
       <c r="A28" s="11" t="s">
         <v>79</v>
       </c>
@@ -1939,14 +1949,14 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="12.8" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="15.5" customWidth="1"/>
-    <col min="2" max="2" width="24.125" customWidth="1"/>
-    <col min="3" max="3" width="25.125" customWidth="1"/>
+    <col min="2" max="2" width="24.1640625" customWidth="1"/>
+    <col min="3" max="3" width="25.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="14.5" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>44</v>
       </c>
@@ -1954,18 +1964,18 @@
         <v>42</v>
       </c>
       <c r="C1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="14.5" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="14.5" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>43</v>
       </c>
@@ -1973,17 +1983,17 @@
         <v>20140227</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="14.5" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>52</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:3" ht="14.6" customHeight="1" x14ac:dyDescent="0.2"/>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="14.5" customHeight="1"/>
+    <row r="6" spans="1:3" ht="14.5" customHeight="1"/>
+    <row r="7" spans="1:3" ht="14.5" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -2002,20 +2012,20 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="5" width="15.375" customWidth="1"/>
+    <col min="1" max="5" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" s="17" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D1" s="17" t="s">
         <v>0</v>
@@ -2024,24 +2034,29 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="E2" s="18" t="s">
         <v>118</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>120</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>121</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>